<commit_message>
- modifying test cases to pass - change in logic of processing the cell value during dt parsing - changes in test data - changes in way how the decision logic element is identified in a worksheet; the 2nd cell describes the type of logic element for a few cases
</commit_message>
<xml_diff>
--- a/test/data/ApplicantData.xlsx
+++ b/test/data/ApplicantData.xlsx
@@ -138,9 +138,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -428,7 +427,7 @@
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,56 +437,57 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>51</v>
       </c>
-      <c r="D3" s="5"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4" t="b">
+      <c r="C6" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="D6" s="5"/>
+      <c r="D6" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>